<commit_message>
Added dotenv file for email and password. Also added a separate file for body and subject text
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Email address</t>
   </si>
@@ -28,13 +28,10 @@
     <t xml:space="preserve">Name (ex. Dela Cruz, Juan Miguel F.)</t>
   </si>
   <si>
-    <t xml:space="preserve">christliebestes@gmail.com</t>
+    <t xml:space="preserve">20190016936@my.xu.edu.ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Christlie Dhon Bestes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Jilhaney</t>
+    <t xml:space="preserve">Josh Paculba</t>
   </si>
 </sst>
 </file>
@@ -152,10 +149,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.32"/>
@@ -172,7 +169,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -181,17 +178,12 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="christliebestes@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fixed base64 encoding when sending certificates
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">Name (ex. Dela Cruz, Juan Miguel F.)</t>
   </si>
   <si>
-    <t xml:space="preserve">20190016936@my.xu.edu.ph</t>
+    <t xml:space="preserve">20190016830@my.xu.edu.ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Josh Paculba</t>
+    <t xml:space="preserve">James Jilhaney</t>
   </si>
 </sst>
 </file>
@@ -114,16 +114,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,7 +144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -149,38 +153,41 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="20190016830@my.xu.edu.ph"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>